<commit_message>
Further additions to bats file builder; started analysis file, tested some first models.
</commit_message>
<xml_diff>
--- a/data/Turbine coordinates 2013 and 2014.xlsx
+++ b/data/Turbine coordinates 2013 and 2014.xlsx
@@ -16,26 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="48">
-  <si>
-    <t>Mid Cambushinnie Farm</t>
-  </si>
-  <si>
-    <t>Letham Farm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="49">
   <si>
     <t>Wester Essendy</t>
   </si>
   <si>
-    <t>Ferrygate Steading</t>
-  </si>
-  <si>
-    <t>Annfield Farm</t>
-  </si>
-  <si>
-    <t>Brockhouse Farm</t>
-  </si>
-  <si>
     <t>Arnbeg Kippen</t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>Huxton</t>
   </si>
   <si>
-    <t>Islabank House</t>
-  </si>
-  <si>
     <t>West Lodge Balmule</t>
   </si>
   <si>
@@ -160,6 +142,27 @@
   </si>
   <si>
     <t>Mid</t>
+  </si>
+  <si>
+    <t>Annfield</t>
+  </si>
+  <si>
+    <t>Brockhouse</t>
+  </si>
+  <si>
+    <t>Ferrygate</t>
+  </si>
+  <si>
+    <t>Islabank</t>
+  </si>
+  <si>
+    <t>Letham Near South T1</t>
+  </si>
+  <si>
+    <t>Letham Far North T2</t>
+  </si>
+  <si>
+    <t>Mid Cambushinnie</t>
   </si>
 </sst>
 </file>
@@ -524,51 +527,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>55.969238299099999</v>
@@ -585,13 +588,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>55.969238299099999</v>
@@ -608,13 +611,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>56.125113611099998</v>
@@ -631,13 +634,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>56.125113611099998</v>
@@ -654,13 +657,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>56.601445950299997</v>
@@ -677,13 +680,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D7">
         <v>56.601029050500003</v>
@@ -700,13 +703,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>56.600665894400002</v>
@@ -723,13 +726,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>56.601029050500003</v>
@@ -746,13 +749,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>56.224153535399999</v>
@@ -769,13 +772,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>56.224153535399999</v>
@@ -792,13 +795,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>56.3299804348</v>
@@ -815,13 +818,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D13">
         <v>56.330098329199998</v>
@@ -838,13 +841,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>56.330039485900002</v>
@@ -861,13 +864,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>56.042152630499999</v>
@@ -884,13 +887,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>56.0419049164</v>
@@ -907,13 +910,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>56.041620357500001</v>
@@ -930,13 +933,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D18">
         <v>56.0419049164</v>
@@ -953,13 +956,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>55.951160928599997</v>
@@ -976,13 +979,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>55.950961493800001</v>
@@ -999,13 +1002,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>55.951061253799999</v>
@@ -1022,13 +1025,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D22">
         <v>55.945460877000002</v>
@@ -1045,13 +1048,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>55.945460877000002</v>
@@ -1068,13 +1071,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D24">
         <v>56.030185639199999</v>
@@ -1091,13 +1094,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D25">
         <v>56.029872706799999</v>
@@ -1114,13 +1117,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>56.030042498699999</v>
@@ -1137,13 +1140,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D27">
         <v>55.9987176092</v>
@@ -1160,13 +1163,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D28">
         <v>55.9987176092</v>
@@ -1183,13 +1186,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D29">
         <v>55.9586823972</v>
@@ -1206,13 +1209,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D30">
         <v>55.9586823972</v>
@@ -1229,13 +1232,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D31">
         <v>56.557220081200001</v>
@@ -1252,13 +1255,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <v>56.557220081200001</v>
@@ -1275,13 +1278,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D33">
         <v>56.094874835799999</v>
@@ -1298,13 +1301,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D34">
         <v>56.094874835799999</v>
@@ -1321,13 +1324,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D35">
         <v>55.885409731499998</v>
@@ -1344,13 +1347,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D36">
         <v>55.885363731399998</v>
@@ -1367,13 +1370,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D37">
         <v>55.885382149500003</v>
@@ -1390,13 +1393,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D38">
         <v>56.064728781399999</v>
@@ -1413,13 +1416,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D39">
         <v>56.064728781399999</v>
@@ -1436,13 +1439,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D40">
         <v>56.357260009900003</v>
@@ -1459,13 +1462,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D41">
         <v>56.357260009900003</v>
@@ -1482,13 +1485,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D42">
         <v>56.250726585899997</v>
@@ -1505,13 +1508,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D43">
         <v>56.250726585899997</v>
@@ -1528,13 +1531,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D44">
         <v>55.909070208300001</v>
@@ -1551,13 +1554,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D45">
         <v>55.908966325999998</v>
@@ -1574,13 +1577,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D46">
         <v>55.909018174099998</v>
@@ -1597,13 +1600,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D47">
         <v>56.079432763</v>
@@ -1620,13 +1623,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D48">
         <v>56.079432763</v>
@@ -1643,13 +1646,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D49">
         <v>56.317717713199997</v>
@@ -1666,13 +1669,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D50">
         <v>56.317410623699999</v>
@@ -1689,13 +1692,13 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D51">
         <v>56.083078567900003</v>
@@ -1712,13 +1715,13 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D52">
         <v>56.083078567900003</v>
@@ -1735,13 +1738,13 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D53" s="2">
         <v>56.066020000000002</v>
@@ -1758,13 +1761,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D54">
         <v>56.066017356899998</v>
@@ -1781,13 +1784,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D55" s="5">
         <v>55.619935010500001</v>
@@ -1804,13 +1807,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D56">
         <v>55.619944009900003</v>
@@ -1827,13 +1830,13 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D57" s="2">
         <v>55.887770000000003</v>
@@ -1850,13 +1853,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D58" s="2">
         <v>55.888069999999999</v>
@@ -1873,13 +1876,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D59">
         <v>56.357260009900003</v>
@@ -1896,13 +1899,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D60" s="2">
         <v>55.743229999999997</v>
@@ -1919,13 +1922,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D61" s="2">
         <v>55.743229999999997</v>
@@ -1942,13 +1945,13 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D62" s="2">
         <v>56.04645</v>
@@ -1965,13 +1968,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D63">
         <v>56.046447898700002</v>
@@ -1988,13 +1991,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D64" s="8">
         <v>55.889710000000001</v>
@@ -2011,13 +2014,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D65" s="8">
         <v>55.889719999999997</v>
@@ -2034,13 +2037,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D66">
         <v>55.889713433399997</v>
@@ -2057,10 +2060,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>41</v>
@@ -2080,180 +2083,180 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="2">
-        <v>56.29072</v>
-      </c>
-      <c r="E68" s="2">
-        <v>-3.3765000000000001</v>
+        <v>35</v>
+      </c>
+      <c r="D68" s="7">
+        <v>56.286470000000001</v>
+      </c>
+      <c r="E68" s="7">
+        <v>-3.3789699999999998</v>
       </c>
       <c r="F68">
-        <v>711771</v>
+        <v>711301</v>
       </c>
       <c r="G68">
-        <v>314895</v>
+        <v>314733</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="2">
+        <v>56.29072</v>
+      </c>
+      <c r="E69" s="2">
+        <v>-3.3765000000000001</v>
+      </c>
+      <c r="F69">
+        <v>711771</v>
+      </c>
+      <c r="G69">
+        <v>314895</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>47</v>
       </c>
-      <c r="D69">
-        <v>56.288658555600001</v>
-      </c>
-      <c r="E69">
-        <v>-3.3777260505100002</v>
-      </c>
-      <c r="F69" s="3">
-        <v>711543</v>
-      </c>
-      <c r="G69" s="3">
-        <v>314815</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>0</v>
-      </c>
       <c r="B70" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D70" s="2">
-        <v>56.2357791799</v>
+        <v>56.29072</v>
       </c>
       <c r="E70" s="2">
-        <v>-3.9315236317000002</v>
-      </c>
-      <c r="F70" s="10">
-        <v>706482</v>
-      </c>
-      <c r="G70" s="10">
-        <v>280373</v>
+        <v>-3.3765000000000001</v>
+      </c>
+      <c r="F70">
+        <v>711771</v>
+      </c>
+      <c r="G70">
+        <v>314895</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D71" s="2">
-        <v>56.235129999999998</v>
+        <v>56.2357791799</v>
       </c>
       <c r="E71" s="2">
-        <v>-3.9319000000000002</v>
+        <v>-3.9315236317000002</v>
       </c>
       <c r="F71" s="10">
-        <v>706411</v>
+        <v>706482</v>
       </c>
       <c r="G71" s="10">
-        <v>280348</v>
+        <v>280373</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D72" s="2">
-        <v>56.23621</v>
+        <v>56.235129999999998</v>
       </c>
       <c r="E72" s="2">
-        <v>-3.9315000000000002</v>
+        <v>-3.9319000000000002</v>
       </c>
       <c r="F72" s="10">
-        <v>706530</v>
+        <v>706411</v>
       </c>
       <c r="G72" s="10">
-        <v>280376</v>
+        <v>280348</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="10">
+        <v>37</v>
+      </c>
+      <c r="D73" s="2">
+        <v>56.23621</v>
+      </c>
+      <c r="E73" s="2">
+        <v>-3.9315000000000002</v>
+      </c>
+      <c r="F73" s="10">
+        <v>706530</v>
+      </c>
+      <c r="G73" s="10">
+        <v>280376</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="10">
         <v>56.235776435799998</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E74" s="10">
         <v>-3.9315267206</v>
       </c>
-      <c r="F73" s="3">
+      <c r="F74" s="3">
         <v>706482</v>
       </c>
-      <c r="G73" s="3">
+      <c r="G74" s="3">
         <v>280373</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>31</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D74" s="5">
-        <v>55.650286700000002</v>
-      </c>
-      <c r="E74" s="5">
-        <v>-2.7469830000000002</v>
-      </c>
-      <c r="F74" s="3">
-        <v>639892</v>
-      </c>
-      <c r="G74" s="3">
-        <v>353090</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C75" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75">
-        <v>55.650286424900003</v>
-      </c>
-      <c r="E75">
-        <v>-2.7469816098000002</v>
+        <v>35</v>
+      </c>
+      <c r="D75" s="5">
+        <v>55.650286700000002</v>
+      </c>
+      <c r="E75" s="5">
+        <v>-2.7469830000000002</v>
       </c>
       <c r="F75" s="3">
         <v>639892</v>
@@ -2264,183 +2267,183 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D76" s="4">
-        <v>55.747540000000001</v>
-      </c>
-      <c r="E76" s="5">
-        <v>-2.3314400000000002</v>
-      </c>
-      <c r="F76">
-        <v>650512</v>
-      </c>
-      <c r="G76">
-        <v>379292</v>
+      <c r="D76">
+        <v>55.650286424900003</v>
+      </c>
+      <c r="E76">
+        <v>-2.7469816098000002</v>
+      </c>
+      <c r="F76" s="3">
+        <v>639892</v>
+      </c>
+      <c r="G76" s="3">
+        <v>353090</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D77" s="4">
-        <v>55.747920000000001</v>
+        <v>55.747540000000001</v>
       </c>
       <c r="E77" s="5">
-        <v>-2.3318599999999998</v>
+        <v>-2.3314400000000002</v>
       </c>
       <c r="F77">
-        <v>650555</v>
+        <v>650512</v>
       </c>
       <c r="G77">
-        <v>379266</v>
+        <v>379292</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D78" s="4">
-        <v>55.74832</v>
+        <v>55.747920000000001</v>
       </c>
       <c r="E78" s="5">
-        <v>-2.3322400000000001</v>
+        <v>-2.3318599999999998</v>
       </c>
       <c r="F78">
-        <v>650600</v>
+        <v>650555</v>
       </c>
       <c r="G78">
-        <v>379242</v>
+        <v>379266</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D79" s="4">
-        <v>55.748699999999999</v>
+        <v>55.74832</v>
       </c>
       <c r="E79" s="5">
-        <v>-2.3326600000000002</v>
+        <v>-2.3322400000000001</v>
       </c>
       <c r="F79">
-        <v>650642</v>
+        <v>650600</v>
       </c>
       <c r="G79">
-        <v>379216</v>
+        <v>379242</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D80">
-        <v>55.748126875700002</v>
-      </c>
-      <c r="E80">
-        <v>-2.33206718867</v>
-      </c>
-      <c r="F80" s="3">
-        <v>650578</v>
-      </c>
-      <c r="G80" s="3">
-        <v>379253</v>
+        <v>38</v>
+      </c>
+      <c r="D80" s="4">
+        <v>55.748699999999999</v>
+      </c>
+      <c r="E80" s="5">
+        <v>-2.3326600000000002</v>
+      </c>
+      <c r="F80">
+        <v>650642</v>
+      </c>
+      <c r="G80">
+        <v>379216</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D81">
-        <v>56.317564168499999</v>
+        <v>55.748126875700002</v>
       </c>
       <c r="E81">
-        <v>-3.30725614297</v>
+        <v>-2.33206718867</v>
       </c>
       <c r="F81" s="3">
-        <v>714675</v>
+        <v>650578</v>
       </c>
       <c r="G81" s="3">
-        <v>319238</v>
+        <v>379253</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D82" s="2">
-        <v>56.57835</v>
-      </c>
-      <c r="E82" s="2">
-        <v>-3.4068499999999999</v>
-      </c>
-      <c r="F82">
-        <v>743821</v>
-      </c>
-      <c r="G82">
-        <v>313672</v>
+      <c r="D82">
+        <v>56.317564168499999</v>
+      </c>
+      <c r="E82">
+        <v>-3.30725614297</v>
+      </c>
+      <c r="F82" s="3">
+        <v>714675</v>
+      </c>
+      <c r="G82" s="3">
+        <v>319238</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D83" s="2">
-        <v>56.578020000000002</v>
+        <v>56.57835</v>
       </c>
       <c r="E83" s="2">
-        <v>-3.4068399999999999</v>
+        <v>-3.4068499999999999</v>
       </c>
       <c r="F83">
-        <v>743784</v>
+        <v>743821</v>
       </c>
       <c r="G83">
         <v>313672</v>
@@ -2448,22 +2451,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D84" s="2">
-        <v>56.577640000000002</v>
+        <v>56.578020000000002</v>
       </c>
       <c r="E84" s="2">
-        <v>-3.4068299999999998</v>
+        <v>-3.4068399999999999</v>
       </c>
       <c r="F84">
-        <v>743742</v>
+        <v>743784</v>
       </c>
       <c r="G84">
         <v>313672</v>
@@ -2471,93 +2474,116 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D85">
-        <v>56.578019576800003</v>
-      </c>
-      <c r="E85">
-        <v>-3.40684123035</v>
-      </c>
-      <c r="F85" s="6">
-        <v>743784</v>
-      </c>
-      <c r="G85" s="6">
+        <v>37</v>
+      </c>
+      <c r="D85" s="2">
+        <v>56.577640000000002</v>
+      </c>
+      <c r="E85" s="2">
+        <v>-3.4068299999999998</v>
+      </c>
+      <c r="F85">
+        <v>743742</v>
+      </c>
+      <c r="G85">
         <v>313672</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D86" s="4">
-        <v>55.642539999999997</v>
-      </c>
-      <c r="E86" s="5">
-        <v>-2.5100500000000001</v>
-      </c>
-      <c r="F86">
-        <v>638895</v>
-      </c>
-      <c r="G86">
-        <v>367994</v>
+      <c r="D86">
+        <v>56.578019576800003</v>
+      </c>
+      <c r="E86">
+        <v>-3.40684123035</v>
+      </c>
+      <c r="F86" s="6">
+        <v>743784</v>
+      </c>
+      <c r="G86" s="6">
+        <v>313672</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D87" s="4">
-        <v>55.642580000000002</v>
+        <v>55.642539999999997</v>
       </c>
       <c r="E87" s="5">
-        <v>-2.5114800000000002</v>
+        <v>-2.5100500000000001</v>
       </c>
       <c r="F87">
-        <v>638900</v>
+        <v>638895</v>
       </c>
       <c r="G87">
-        <v>367904</v>
+        <v>367994</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D88">
+      <c r="D88" s="4">
+        <v>55.642580000000002</v>
+      </c>
+      <c r="E88" s="5">
+        <v>-2.5114800000000002</v>
+      </c>
+      <c r="F88">
+        <v>638900</v>
+      </c>
+      <c r="G88">
+        <v>367904</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D89">
         <v>55.642557024399999</v>
       </c>
-      <c r="E88">
+      <c r="E89">
         <v>-2.5107466831499998</v>
       </c>
-      <c r="F88" s="3">
+      <c r="F89" s="3">
         <v>638897</v>
       </c>
-      <c r="G88" s="3">
+      <c r="G89" s="3">
         <v>367950</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small updates to tables missing values.
</commit_message>
<xml_diff>
--- a/data/Turbine coordinates 2013 and 2014.xlsx
+++ b/data/Turbine coordinates 2013 and 2014.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="11310"/>
+    <workbookView xWindow="19000" yWindow="0" windowWidth="19360" windowHeight="19500"/>
   </bookViews>
   <sheets>
     <sheet name="Turbine coordinates 2013 and 20" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="50">
   <si>
     <t>Wester Essendy</t>
   </si>
@@ -163,6 +168,9 @@
   </si>
   <si>
     <t>Mid Cambushinnie</t>
+  </si>
+  <si>
+    <t>Turb_height</t>
   </si>
 </sst>
 </file>
@@ -172,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +197,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,8 +235,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -227,7 +253,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,20 +555,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="9"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -562,8 +590,11 @@
       <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -585,8 +616,11 @@
       <c r="G2" s="3">
         <v>349508</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -608,8 +642,11 @@
       <c r="G3" s="3">
         <v>349508</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -631,8 +668,11 @@
       <c r="G4" s="3">
         <v>262942</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -654,8 +694,11 @@
       <c r="G5" s="3">
         <v>262942</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -677,8 +720,11 @@
       <c r="G6" s="3">
         <v>331581</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -700,8 +746,11 @@
       <c r="G7" s="3">
         <v>331617</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -723,8 +772,11 @@
       <c r="G8" s="3">
         <v>331652</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -746,8 +798,11 @@
       <c r="G9" s="3">
         <v>331617</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -769,8 +824,11 @@
       <c r="G10" s="3">
         <v>274746</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -792,8 +850,11 @@
       <c r="G11" s="3">
         <v>274746</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -815,8 +876,11 @@
       <c r="G12" s="3">
         <v>302167</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -838,8 +902,11 @@
       <c r="G13" s="3">
         <v>302216</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -861,8 +928,11 @@
       <c r="G14" s="3">
         <v>302192</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -884,8 +954,11 @@
       <c r="G15" s="3">
         <v>351790</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -907,8 +980,11 @@
       <c r="G16" s="3">
         <v>351828</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -930,8 +1006,11 @@
       <c r="G17" s="3">
         <v>351857</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -953,8 +1032,11 @@
       <c r="G18" s="3">
         <v>351828</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -976,8 +1058,11 @@
       <c r="G19" s="3">
         <v>359314</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -999,8 +1084,11 @@
       <c r="G20" s="3">
         <v>359293</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1022,8 +1110,11 @@
       <c r="G21" s="3">
         <v>359304</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1045,8 +1136,11 @@
       <c r="G22" s="3">
         <v>338313</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1068,8 +1162,11 @@
       <c r="G23" s="3">
         <v>338313</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1091,8 +1188,11 @@
       <c r="G24" s="3">
         <v>352142</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1114,8 +1214,11 @@
       <c r="G25" s="3">
         <v>352157</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1137,8 +1240,11 @@
       <c r="G26" s="3">
         <v>352148</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1160,8 +1266,11 @@
       <c r="G27" s="3">
         <v>354280</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1183,8 +1292,11 @@
       <c r="G28" s="3">
         <v>354280</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1206,8 +1318,11 @@
       <c r="G29" s="3">
         <v>345331</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -1229,8 +1344,11 @@
       <c r="G30" s="3">
         <v>345331</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1252,8 +1370,11 @@
       <c r="G31" s="3">
         <v>319853</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1275,8 +1396,11 @@
       <c r="G32" s="3">
         <v>319853</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1298,8 +1422,11 @@
       <c r="G33" s="3">
         <v>276362</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1321,8 +1448,11 @@
       <c r="G34" s="3">
         <v>276362</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1344,8 +1474,11 @@
       <c r="G35" s="3">
         <v>356790</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1367,8 +1500,11 @@
       <c r="G36" s="1">
         <v>356778</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1390,8 +1526,11 @@
       <c r="G37" s="3">
         <v>356783</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1413,8 +1552,11 @@
       <c r="G38" s="3">
         <v>295223</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1436,8 +1578,11 @@
       <c r="G39" s="3">
         <v>295223</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1459,8 +1604,11 @@
       <c r="G40" s="3">
         <v>294103</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1482,8 +1630,11 @@
       <c r="G41" s="3">
         <v>294103</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1505,8 +1656,11 @@
       <c r="G42" s="3">
         <v>331810</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1528,8 +1682,11 @@
       <c r="G43" s="3">
         <v>331810</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1551,8 +1708,11 @@
       <c r="G44" s="3">
         <v>355084</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1574,8 +1734,11 @@
       <c r="G45" s="3">
         <v>355126</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1597,8 +1760,11 @@
       <c r="G46" s="3">
         <v>355104</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -1620,8 +1786,11 @@
       <c r="G47" s="3">
         <v>274749</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -1643,8 +1812,11 @@
       <c r="G48" s="3">
         <v>274749</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -1666,8 +1838,11 @@
       <c r="G49" s="3">
         <v>319243</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -1689,8 +1864,11 @@
       <c r="G50" s="3">
         <v>319233</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -1712,8 +1890,11 @@
       <c r="G51" s="3">
         <v>320523</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1735,8 +1916,11 @@
       <c r="G52" s="3">
         <v>320523</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -1758,8 +1942,11 @@
       <c r="G53" s="3">
         <v>314566</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -1781,8 +1968,11 @@
       <c r="G54" s="3">
         <v>314566</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -1804,8 +1994,11 @@
       <c r="G55" s="3">
         <v>364617</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -1827,8 +2020,11 @@
       <c r="G56" s="3">
         <v>364617</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -1850,8 +2046,11 @@
       <c r="G57">
         <v>384979</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -1873,8 +2072,11 @@
       <c r="G58">
         <v>384951</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -1896,8 +2098,11 @@
       <c r="G59" s="3">
         <v>384966</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -1919,8 +2124,11 @@
       <c r="G60">
         <v>341782</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -1942,8 +2150,11 @@
       <c r="G61">
         <v>341782</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>44</v>
       </c>
@@ -1965,8 +2176,11 @@
       <c r="G62" s="3">
         <v>352972</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>44</v>
       </c>
@@ -1988,8 +2202,11 @@
       <c r="G63" s="3">
         <v>352972</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -2011,8 +2228,11 @@
       <c r="G64">
         <v>386093</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -2034,8 +2254,11 @@
       <c r="G65">
         <v>386036</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -2057,8 +2280,11 @@
       <c r="G66" s="3">
         <v>386064</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -2080,8 +2306,11 @@
       <c r="G67">
         <v>314733</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>46</v>
       </c>
@@ -2103,8 +2332,11 @@
       <c r="G68">
         <v>314733</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>47</v>
       </c>
@@ -2126,8 +2358,11 @@
       <c r="G69">
         <v>314895</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -2149,8 +2384,11 @@
       <c r="G70">
         <v>314895</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="10" customFormat="1">
       <c r="A71" s="10" t="s">
         <v>48</v>
       </c>
@@ -2172,8 +2410,11 @@
       <c r="G71" s="10">
         <v>280373</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="10" customFormat="1">
       <c r="A72" s="10" t="s">
         <v>48</v>
       </c>
@@ -2195,8 +2436,11 @@
       <c r="G72" s="10">
         <v>280348</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="10" customFormat="1">
       <c r="A73" s="10" t="s">
         <v>48</v>
       </c>
@@ -2218,8 +2462,11 @@
       <c r="G73" s="10">
         <v>280376</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="10" customFormat="1">
       <c r="A74" s="10" t="s">
         <v>48</v>
       </c>
@@ -2241,8 +2488,11 @@
       <c r="G74" s="3">
         <v>280373</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -2264,8 +2514,11 @@
       <c r="G75" s="3">
         <v>353090</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>25</v>
       </c>
@@ -2287,8 +2540,11 @@
       <c r="G76" s="3">
         <v>353090</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -2310,8 +2566,11 @@
       <c r="G77">
         <v>379292</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -2333,8 +2592,11 @@
       <c r="G78">
         <v>379266</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2356,8 +2618,11 @@
       <c r="G79">
         <v>379242</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -2379,8 +2644,11 @@
       <c r="G80">
         <v>379216</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -2402,8 +2670,11 @@
       <c r="G81" s="3">
         <v>379253</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -2425,8 +2696,11 @@
       <c r="G82" s="3">
         <v>319238</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -2448,8 +2722,11 @@
       <c r="G83">
         <v>313672</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2471,8 +2748,11 @@
       <c r="G84">
         <v>313672</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -2494,8 +2774,11 @@
       <c r="G85">
         <v>313672</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -2517,8 +2800,11 @@
       <c r="G86" s="6">
         <v>313672</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -2540,8 +2826,11 @@
       <c r="G87">
         <v>367994</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -2563,8 +2852,11 @@
       <c r="G88">
         <v>367904</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -2585,6 +2877,9 @@
       </c>
       <c r="G89" s="3">
         <v>367950</v>
+      </c>
+      <c r="H89">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2592,7 +2887,12 @@
     <sortCondition ref="A2:A88"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2602,9 +2902,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2614,8 +2919,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>